<commit_message>
ajout du datapath de l'instruction jal dans le schema et des CU codes dans la table de verite
</commit_message>
<xml_diff>
--- a/table-de-verite.xlsx
+++ b/table-de-verite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\University\AUT18\IFT1227\IFT1227---ProcessorMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B15B56F7-B50A-477A-B8DF-3330D1D6CAAD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5189813-0B33-4111-8CDF-0472EBB98775}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3990" xr2:uid="{E11BBDBF-22C9-4E1A-B687-3EF699DDACB4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Op[5:0]</t>
   </si>
@@ -132,13 +132,19 @@
   </si>
   <si>
     <t>ALUsrc</t>
+  </si>
+  <si>
+    <t>jal</t>
+  </si>
+  <si>
+    <t>000011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +162,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF78E25"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,19 +194,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF78E25"/>
+      <color rgb="FF1705C7"/>
+      <color rgb="FF7DF307"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -502,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC0858-4C72-42D9-9567-FEE4A5228686}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +536,7 @@
     <col min="8" max="8" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -546,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -556,8 +578,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -568,8 +590,8 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -578,7 +600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -588,8 +610,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>30</v>
@@ -600,8 +622,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="H3" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>13</v>
@@ -610,7 +632,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -620,7 +642,7 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -632,7 +654,7 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -642,7 +664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -652,7 +674,7 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -664,7 +686,7 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -674,7 +696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -684,7 +706,7 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -696,7 +718,7 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
@@ -706,7 +728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -716,8 +738,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>30</v>
@@ -728,8 +750,8 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>0</v>
+      <c r="H7" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>13</v>
@@ -738,7 +760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -748,8 +770,8 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>27</v>
@@ -760,8 +782,8 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>28</v>
@@ -770,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -802,7 +824,44 @@
         <v>27</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G14" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout des data paths de slt et sll, ajout des codes du CU dans la table de verite
</commit_message>
<xml_diff>
--- a/table-de-verite.xlsx
+++ b/table-de-verite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\University\AUT18\IFT1227\IFT1227---ProcessorMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5189813-0B33-4111-8CDF-0472EBB98775}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36165588-5D25-4222-B568-54738D8587E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3990" xr2:uid="{E11BBDBF-22C9-4E1A-B687-3EF699DDACB4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>Op[5:0]</t>
   </si>
@@ -138,13 +138,28 @@
   </si>
   <si>
     <t>000011</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>slt</t>
+  </si>
+  <si>
+    <t>101010</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +188,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF996633"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,6 +232,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,6 +244,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF996633"/>
+      <color rgb="FFFFFF00"/>
       <color rgb="FFF78E25"/>
       <color rgb="FF1705C7"/>
       <color rgb="FF7DF307"/>
@@ -527,7 +562,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,7 +832,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -856,6 +891,68 @@
         <v>30</v>
       </c>
       <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G14" s="6"/>

</xml_diff>

<commit_message>
Final commit de la journee, il reste lb,slt et lui a faire pour demain
</commit_message>
<xml_diff>
--- a/table-de-verite.xlsx
+++ b/table-de-verite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\University\AUT18\IFT1227\IFT1227---ProcessorMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36165588-5D25-4222-B568-54738D8587E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1258A8-CAC2-49C6-B4B8-BCC63C6CE4F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3990" xr2:uid="{E11BBDBF-22C9-4E1A-B687-3EF699DDACB4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
   <si>
     <t>Op[5:0]</t>
   </si>
@@ -143,23 +143,38 @@
     <t>sll</t>
   </si>
   <si>
-    <t>slt</t>
-  </si>
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
     <t>00000</t>
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>ori</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>001101</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>XXXXX</t>
+  </si>
+  <si>
+    <t>sltu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +217,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1705C7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,6 +258,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,10 +268,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1705C7"/>
       <color rgb="FF996633"/>
       <color rgb="FFFFFF00"/>
       <color rgb="FFF78E25"/>
-      <color rgb="FF1705C7"/>
       <color rgb="FF7DF307"/>
     </mruColors>
   </colors>
@@ -559,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC0858-4C72-42D9-9567-FEE4A5228686}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,8 +634,8 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>30</v>
@@ -619,11 +643,11 @@
       <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>29</v>
@@ -642,8 +666,8 @@
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>29</v>
@@ -651,11 +675,11 @@
       <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>30</v>
@@ -674,23 +698,23 @@
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -706,23 +730,23 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>19</v>
@@ -738,26 +762,26 @@
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>30</v>
@@ -770,8 +794,8 @@
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>29</v>
@@ -779,11 +803,11 @@
       <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>29</v>
@@ -802,8 +826,8 @@
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>29</v>
@@ -811,11 +835,11 @@
       <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
+      <c r="F8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>29</v>
@@ -832,28 +856,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
+      <c r="G9" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>27</v>
@@ -866,26 +890,26 @@
       <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6">
-        <v>1</v>
+      <c r="C10" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="6">
-        <v>0</v>
+      <c r="G10" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>30</v>
@@ -894,13 +918,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1</v>
+      <c r="C11" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>30</v>
@@ -908,17 +932,17 @@
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
+      <c r="F11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>29</v>
@@ -929,20 +953,22 @@
         <v>36</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="D12" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="10">
-        <v>0</v>
-      </c>
-      <c r="G12" s="10">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>29</v>
@@ -954,8 +980,43 @@
         <v>29</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G14" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>